<commit_message>
V1.0_beta prototype. Firwmare fixes
</commit_message>
<xml_diff>
--- a/gerbers/Pi-pico-AD9854_BOM.xlsx
+++ b/gerbers/Pi-pico-AD9854_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98410007bacd207f/Matteo/KiCad/Circuits/Pi-pico-AD9854_adapter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/m_mazzanti_uva_nl/Documents/Documents/GitHub/PicoDDS/gerbers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{7BE910D2-B302-4CA2-A65F-3AA2A1011AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A462B779-91DB-4EEB-BBEF-01F76BA1C714}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{7BE910D2-B302-4CA2-A65F-3AA2A1011AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2E3EDBE-D33D-4568-8CE9-6E8ACC331E52}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{39FF018D-9061-4871-861C-5D5002EE47BB}"/>
+    <workbookView xWindow="2478" yWindow="204" windowWidth="17280" windowHeight="8994" xr2:uid="{39FF018D-9061-4871-861C-5D5002EE47BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Comment</t>
   </si>
@@ -111,18 +111,9 @@
     <t>C130397</t>
   </si>
   <si>
-    <t>LM3940IMP-3.3/NOPB</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
-    <t>SOT-223</t>
-  </si>
-  <si>
-    <t>C140319</t>
-  </si>
-  <si>
     <t>SMB,DO-214AA</t>
   </si>
   <si>
@@ -157,6 +148,12 @@
   </si>
   <si>
     <t>C150470</t>
+  </si>
+  <si>
+    <t>C662441</t>
+  </si>
+  <si>
+    <t>LT1086IM-3.3#TRPBF</t>
   </si>
 </sst>
 </file>
@@ -520,18 +517,18 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.58984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.9453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -559,7 +556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -573,7 +570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -581,41 +578,41 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -629,7 +626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -643,7 +640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -657,7 +654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>0</v>
       </c>
@@ -671,32 +668,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
       <c r="D11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>